<commit_message>
updated files from tufts 4/25
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/BDbDT/BAU Deaths by Demographic Trait.xlsx
+++ b/InputData/add-outputs/BDbDT/BAU Deaths by Demographic Trait.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\Indonesia\eps-indonesia\InputData\add-outputs\BDbDT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\add-outputs\BDbDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D09D698-B00B-443B-80C7-F77A11AF4E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6893DD55-4A20-4421-8A92-C311A477EB68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="20040" windowHeight="14565" activeTab="2" xr2:uid="{07D21EFD-220B-4C60-85BD-FCD4C246A818}"/>
+    <workbookView xWindow="11760" yWindow="1410" windowWidth="23970" windowHeight="20745" xr2:uid="{07D21EFD-220B-4C60-85BD-FCD4C246A818}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -523,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66936CFD-0A84-4062-AAF5-5F189C33D342}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19215,9 +19215,7 @@
   </sheetPr>
   <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AF9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19324,97 +19322,128 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,B$1)</f>
+        <v>1399014</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,C$1)</f>
+        <v>1415904</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,D$1)</f>
+        <v>1433335</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,E$1)</f>
+        <v>1451474</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,F$1)</f>
+        <v>1470351</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,G$1)</f>
+        <v>1490023</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,H$1)</f>
+        <v>1510466</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,I$1)</f>
+        <v>1531731</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,J$1)</f>
+        <v>1553790</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,K$1)</f>
+        <v>1576409</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,L$1)</f>
+        <v>1599622</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,M$1)</f>
+        <v>1623126</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,N$1)</f>
+        <v>1646815</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,O$1)</f>
+        <v>1670459</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,P$1)</f>
+        <v>1693916</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,Q$1)</f>
+        <v>1717014</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,R$1)</f>
+        <v>1739536</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,S$1)</f>
+        <v>1761331</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,T$1)</f>
+        <v>1782074</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,U$1)</f>
+        <v>1801727</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,V$1)</f>
+        <v>1820048</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,W$1)</f>
+        <v>1836978</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,X$1)</f>
+        <v>1852429</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,Y$1)</f>
+        <v>1866421</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,Z$1)</f>
+        <v>1878578</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,AA$1)</f>
+        <v>1889035</v>
       </c>
       <c r="AB2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,AB$1)</f>
+        <v>1897754</v>
       </c>
       <c r="AC2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,AC$1)</f>
+        <v>1905227</v>
       </c>
       <c r="AD2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,AD$1)</f>
+        <v>1911162</v>
       </c>
       <c r="AE2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,AE$1)</f>
+        <v>1915462</v>
       </c>
       <c r="AF2">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,1,'Census T3'!$C:$C,AF$1)</f>
+        <v>1918329</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
@@ -19422,97 +19451,128 @@
         <v>26</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,B$1)</f>
+        <v>1352797</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,C$1)</f>
+        <v>1364899</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,D$1)</f>
+        <v>1378001</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,E$1)</f>
+        <v>1392289</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,F$1)</f>
+        <v>1407974</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,G$1)</f>
+        <v>1425115</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,H$1)</f>
+        <v>1443782</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,I$1)</f>
+        <v>1464109</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,J$1)</f>
+        <v>1486000</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,K$1)</f>
+        <v>1509417</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,L$1)</f>
+        <v>1534253</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,M$1)</f>
+        <v>1560453</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,N$1)</f>
+        <v>1587775</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,O$1)</f>
+        <v>1616042</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,P$1)</f>
+        <v>1644942</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,Q$1)</f>
+        <v>1674402</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,R$1)</f>
+        <v>1704021</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,S$1)</f>
+        <v>1733397</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,T$1)</f>
+        <v>1762454</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,U$1)</f>
+        <v>1790640</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,V$1)</f>
+        <v>1817830</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,W$1)</f>
+        <v>1843670</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,X$1)</f>
+        <v>1868030</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,Y$1)</f>
+        <v>1890872</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,Z$1)</f>
+        <v>1911722</v>
       </c>
       <c r="AA3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,AA$1)</f>
+        <v>1930252</v>
       </c>
       <c r="AB3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,AB$1)</f>
+        <v>1946383</v>
       </c>
       <c r="AC3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,AC$1)</f>
+        <v>1961288</v>
       </c>
       <c r="AD3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,AD$1)</f>
+        <v>1973949</v>
       </c>
       <c r="AE3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,AE$1)</f>
+        <v>1984222</v>
       </c>
       <c r="AF3">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,2,'Census T3'!$C:$C,AF$1)</f>
+        <v>1992132</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
@@ -19520,97 +19580,128 @@
         <v>28</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,B$1)</f>
+        <v>2266508</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,C$1)</f>
+        <v>2288372</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,D$1)</f>
+        <v>2311305</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,E$1)</f>
+        <v>2335658</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,F$1)</f>
+        <v>2361634</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,G$1)</f>
+        <v>2389358</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,H$1)</f>
+        <v>2418894</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,I$1)</f>
+        <v>2450373</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,J$1)</f>
+        <v>2483710</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,K$1)</f>
+        <v>2518661</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,L$1)</f>
+        <v>2555182</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,M$1)</f>
+        <v>2592915</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,N$1)</f>
+        <v>2631544</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,O$1)</f>
+        <v>2670665</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,P$1)</f>
+        <v>2709880</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Q$1)</f>
+        <v>2749028</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,R$1)</f>
+        <v>2787487</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,S$1)</f>
+        <v>2824803</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,T$1)</f>
+        <v>2860661</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,U$1)</f>
+        <v>2894554</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,V$1)</f>
+        <v>2926113</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,W$1)</f>
+        <v>2955004</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,X$1)</f>
+        <v>2981129</v>
       </c>
       <c r="Y4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Y$1)</f>
+        <v>3004515</v>
       </c>
       <c r="Z4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Z$1)</f>
+        <v>3024344</v>
       </c>
       <c r="AA4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AA$1)</f>
+        <v>3040446</v>
       </c>
       <c r="AB4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AB$1)</f>
+        <v>3052853</v>
       </c>
       <c r="AC4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AC$1)</f>
+        <v>3063089</v>
       </c>
       <c r="AD4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AD$1)</f>
+        <v>3069927</v>
       </c>
       <c r="AE4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AE$1)</f>
+        <v>3073176</v>
       </c>
       <c r="AF4">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,1,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AF$1)</f>
+        <v>3073035</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -19618,97 +19709,128 @@
         <v>29</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,B$1)</f>
+        <v>332414</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,C$1)</f>
+        <v>335694</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,D$1)</f>
+        <v>339204</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,E$1)</f>
+        <v>342968</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,F$1)</f>
+        <v>346991</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,G$1)</f>
+        <v>351241</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,H$1)</f>
+        <v>355775</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,I$1)</f>
+        <v>360569</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,J$1)</f>
+        <v>365554</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,K$1)</f>
+        <v>370799</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,L$1)</f>
+        <v>376278</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,M$1)</f>
+        <v>381963</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,N$1)</f>
+        <v>387899</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,O$1)</f>
+        <v>394000</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,P$1)</f>
+        <v>400324</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Q$1)</f>
+        <v>406761</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,R$1)</f>
+        <v>413354</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,S$1)</f>
+        <v>420015</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,T$1)</f>
+        <v>426673</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,U$1)</f>
+        <v>433341</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,V$1)</f>
+        <v>439962</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,W$1)</f>
+        <v>446507</v>
       </c>
       <c r="X5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,X$1)</f>
+        <v>452925</v>
       </c>
       <c r="Y5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Y$1)</f>
+        <v>459140</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Z$1)</f>
+        <v>465151</v>
       </c>
       <c r="AA5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AA$1)</f>
+        <v>470941</v>
       </c>
       <c r="AB5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AB$1)</f>
+        <v>476368</v>
       </c>
       <c r="AC5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AC$1)</f>
+        <v>481543</v>
       </c>
       <c r="AD5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AD$1)</f>
+        <v>486451</v>
       </c>
       <c r="AE5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AE$1)</f>
+        <v>490963</v>
       </c>
       <c r="AF5">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,2,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AF$1)</f>
+        <v>495178</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
@@ -19716,97 +19838,128 @@
         <v>30</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,B$1)</f>
+        <v>97716</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,C$1)</f>
+        <v>100313</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,D$1)</f>
+        <v>103074</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,E$1)</f>
+        <v>106023</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,F$1)</f>
+        <v>109158</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,G$1)</f>
+        <v>112427</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,H$1)</f>
+        <v>115918</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,I$1)</f>
+        <v>119579</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,J$1)</f>
+        <v>123436</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,K$1)</f>
+        <v>127462</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,L$1)</f>
+        <v>131643</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,M$1)</f>
+        <v>135991</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,N$1)</f>
+        <v>140437</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,O$1)</f>
+        <v>145048</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,P$1)</f>
+        <v>149744</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Q$1)</f>
+        <v>154546</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,R$1)</f>
+        <v>159416</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,S$1)</f>
+        <v>164345</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,T$1)</f>
+        <v>169315</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,U$1)</f>
+        <v>174279</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,V$1)</f>
+        <v>179269</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,W$1)</f>
+        <v>184204</v>
       </c>
       <c r="X6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,X$1)</f>
+        <v>189142</v>
       </c>
       <c r="Y6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Y$1)</f>
+        <v>193999</v>
       </c>
       <c r="Z6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Z$1)</f>
+        <v>198834</v>
       </c>
       <c r="AA6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AA$1)</f>
+        <v>203605</v>
       </c>
       <c r="AB6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AB$1)</f>
+        <v>208294</v>
       </c>
       <c r="AC6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AC$1)</f>
+        <v>212958</v>
       </c>
       <c r="AD6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AD$1)</f>
+        <v>217538</v>
       </c>
       <c r="AE6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AE$1)</f>
+        <v>222072</v>
       </c>
       <c r="AF6">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,4,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AF$1)</f>
+        <v>226577</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
@@ -19814,97 +19967,128 @@
         <v>31</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,B$1)-SUM(B4:B6)</f>
+        <v>55173</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,C$1)-SUM(C4:C6)</f>
+        <v>56424</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,D$1)-SUM(D4:D6)</f>
+        <v>57753</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,E$1)-SUM(E4:E6)</f>
+        <v>59114</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,F$1)-SUM(F4:F6)</f>
+        <v>60542</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,G$1)-SUM(G4:G6)</f>
+        <v>62112</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,H$1)-SUM(H4:H6)</f>
+        <v>63661</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,I$1)-SUM(I4:I6)</f>
+        <v>65319</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,J$1)-SUM(J4:J6)</f>
+        <v>67090</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,K$1)-SUM(K4:K6)</f>
+        <v>68904</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,L$1)-SUM(L4:L6)</f>
+        <v>70772</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,M$1)-SUM(M4:M6)</f>
+        <v>72710</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,N$1)-SUM(N4:N6)</f>
+        <v>74710</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,O$1)-SUM(O4:O6)</f>
+        <v>76788</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,P$1)-SUM(P4:P6)</f>
+        <v>78910</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Q$1)-SUM(Q4:Q6)</f>
+        <v>81081</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,R$1)-SUM(R4:R6)</f>
+        <v>83300</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,S$1)-SUM(S4:S6)</f>
+        <v>85565</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,T$1)-SUM(T4:T6)</f>
+        <v>87879</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,U$1)-SUM(U4:U6)</f>
+        <v>90193</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,V$1)-SUM(V4:V6)</f>
+        <v>92534</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,W$1)-SUM(W4:W6)</f>
+        <v>94933</v>
       </c>
       <c r="X7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,X$1)-SUM(X4:X6)</f>
+        <v>97263</v>
       </c>
       <c r="Y7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Y$1)-SUM(Y4:Y6)</f>
+        <v>99639</v>
       </c>
       <c r="Z7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Z$1)-SUM(Z4:Z6)</f>
+        <v>101971</v>
       </c>
       <c r="AA7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AA$1)-SUM(AA4:AA6)</f>
+        <v>104295</v>
       </c>
       <c r="AB7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AB$1)-SUM(AB4:AB6)</f>
+        <v>106622</v>
       </c>
       <c r="AC7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AC$1)-SUM(AC4:AC6)</f>
+        <v>108925</v>
       </c>
       <c r="AD7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AD$1)-SUM(AD4:AD6)</f>
+        <v>111195</v>
       </c>
       <c r="AE7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AE$1)-SUM(AE4:AE6)</f>
+        <v>113473</v>
       </c>
       <c r="AF7">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AF$1)-SUM(AF4:AF6)</f>
+        <v>115671</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
@@ -19912,97 +20096,128 @@
         <v>32</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,B$1)</f>
+        <v>218889</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,C$1)</f>
+        <v>225675</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,D$1)</f>
+        <v>232814</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,E$1)</f>
+        <v>240210</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,F$1)</f>
+        <v>247965</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,G$1)</f>
+        <v>256017</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,H$1)</f>
+        <v>264411</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,I$1)</f>
+        <v>273169</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,J$1)</f>
+        <v>282334</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,K$1)</f>
+        <v>291883</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,L$1)</f>
+        <v>301878</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,M$1)</f>
+        <v>312190</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,N$1)</f>
+        <v>322962</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,O$1)</f>
+        <v>334098</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,P$1)</f>
+        <v>345580</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Q$1)</f>
+        <v>357514</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,R$1)</f>
+        <v>369815</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,S$1)</f>
+        <v>382416</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,T$1)</f>
+        <v>395312</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,U$1)</f>
+        <v>408544</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,V$1)</f>
+        <v>422047</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,W$1)</f>
+        <v>435734</v>
       </c>
       <c r="X8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,X$1)</f>
+        <v>449637</v>
       </c>
       <c r="Y8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Y$1)</f>
+        <v>463744</v>
       </c>
       <c r="Z8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Z$1)</f>
+        <v>477956</v>
       </c>
       <c r="AA8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AA$1)</f>
+        <v>492266</v>
       </c>
       <c r="AB8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AB$1)</f>
+        <v>506629</v>
       </c>
       <c r="AC8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AC$1)</f>
+        <v>521040</v>
       </c>
       <c r="AD8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AD$1)</f>
+        <v>535466</v>
       </c>
       <c r="AE8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AE$1)</f>
+        <v>549807</v>
       </c>
       <c r="AF8">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,8,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AF$1)</f>
+        <v>564105</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
@@ -20010,97 +20225,128 @@
         <v>33</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,B$1)-B8</f>
+        <v>2532922</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,C$1)-C8</f>
+        <v>2555128</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,D$1)-D8</f>
+        <v>2578522</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,E$1)-E8</f>
+        <v>2603553</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,F$1)-F8</f>
+        <v>2630360</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,G$1)-G8</f>
+        <v>2659121</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,H$1)-H8</f>
+        <v>2689837</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,I$1)-I8</f>
+        <v>2722671</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,J$1)-J8</f>
+        <v>2757456</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,K$1)-K8</f>
+        <v>2793943</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,L$1)-L8</f>
+        <v>2831997</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,M$1)-M8</f>
+        <v>2871389</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,N$1)-N8</f>
+        <v>2911628</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,O$1)-O8</f>
+        <v>2952403</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,P$1)-P8</f>
+        <v>2993278</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Q$1)-Q8</f>
+        <v>3033902</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,R$1)-R8</f>
+        <v>3073742</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,S$1)-S8</f>
+        <v>3112312</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,T$1)-T8</f>
+        <v>3149216</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,U$1)-U8</f>
+        <v>3183823</v>
       </c>
       <c r="V9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,V$1)-V8</f>
+        <v>3215831</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,W$1)-W8</f>
+        <v>3244914</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,X$1)-X8</f>
+        <v>3270822</v>
       </c>
       <c r="Y9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Y$1)-Y8</f>
+        <v>3293549</v>
       </c>
       <c r="Z9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,Z$1)-Z8</f>
+        <v>3312344</v>
       </c>
       <c r="AA9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AA$1)-AA8</f>
+        <v>3327021</v>
       </c>
       <c r="AB9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AB$1)-AB8</f>
+        <v>3337508</v>
       </c>
       <c r="AC9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AC$1)-AC8</f>
+        <v>3345475</v>
       </c>
       <c r="AD9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AD$1)-AD8</f>
+        <v>3349645</v>
       </c>
       <c r="AE9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AE$1)-AE8</f>
+        <v>3349877</v>
       </c>
       <c r="AF9">
-        <v>0</v>
+        <f>SUMIFS('Census T3'!$D:$D,'Census T3'!$A:$A,0,'Census T3'!$B:$B,0,'Census T3'!$C:$C,AF$1)-AF8</f>
+        <v>3346356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>